<commit_message>
Platinum Video Carousel Update
</commit_message>
<xml_diff>
--- a/polls/ICRA20Sponsors.xlsx
+++ b/polls/ICRA20Sponsors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5F3601-AF09-484F-9B82-B44B5484C154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AEF432-986D-4C15-96DA-58FD17DAA989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99C90C33-A2F8-49BC-95C2-22A337B4C8DB}"/>
   </bookViews>
@@ -71,15 +71,6 @@
     <t>Video</t>
   </si>
   <si>
-    <t>Aerial Systems - Application I</t>
-  </si>
-  <si>
-    <t>Aerial Systems - Application II</t>
-  </si>
-  <si>
-    <t>Aerial Systems - Application III</t>
-  </si>
-  <si>
     <t>Legged Robots I</t>
   </si>
   <si>
@@ -96,6 +87,15 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Aerial Systems - Applications I</t>
+  </si>
+  <si>
+    <t>Aerial Systems - Applications II</t>
+  </si>
+  <si>
+    <t>Aerial Systems - Applications III</t>
   </si>
 </sst>
 </file>
@@ -464,14 +464,14 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="3" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
@@ -482,13 +482,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -526,7 +526,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -554,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -568,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -582,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -596,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -610,7 +610,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
View Count and Bug fix
Login function is left
</commit_message>
<xml_diff>
--- a/polls/ICRA20Sponsors.xlsx
+++ b/polls/ICRA20Sponsors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AEF432-986D-4C15-96DA-58FD17DAA989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBBD375-6C9A-44C9-A3F6-AB4E814665C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99C90C33-A2F8-49BC-95C2-22A337B4C8DB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Cartegory</t>
   </si>
@@ -96,13 +96,28 @@
   </si>
   <si>
     <t>Aerial Systems - Applications III</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.dji.com/</t>
+  </si>
+  <si>
+    <t>https://www.skydio.com/</t>
+  </si>
+  <si>
+    <t>http://pal-robotics.com/</t>
+  </si>
+  <si>
+    <t>https://www.bostondynamics.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +128,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
@@ -136,10 +160,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,9 +172,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -461,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE3CA7B-2F7F-49E8-81CC-0A8442F28240}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -477,7 +507,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +520,11 @@
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -507,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -515,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -528,8 +561,11 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -542,8 +578,11 @@
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -556,8 +595,11 @@
       <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -570,8 +612,11 @@
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -584,8 +629,11 @@
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -598,8 +646,11 @@
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -612,25 +663,37 @@
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{208568F0-3478-4D37-84B1-9B721CD8244C}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{88891F5E-3CE8-40D8-9919-39AC62289DCA}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{B193D66D-911F-4E49-ACB7-0594743D2D1E}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{100AE16B-A6AB-4FBA-BBE2-A223763ACBA5}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{B0CF259C-6270-4913-9E01-30C0433BE84A}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{2C15309B-98DA-49A8-AD87-DDA45F02F1CF}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{127C49E7-6F2B-4E7E-B04E-95FE6D34B74D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>